<commit_message>
Adjustment sensitivity EOL RIR
</commit_message>
<xml_diff>
--- a/Results/Sensitivity/EOL-RIR/Lifetime/EOL_RIR_full_Lifetime_Avg.xlsx
+++ b/Results/Sensitivity/EOL-RIR/Lifetime/EOL_RIR_full_Lifetime_Avg.xlsx
@@ -397,7 +397,7 @@
         <v>2011</v>
       </c>
       <c r="C1" s="1">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1">
         <v>2050</v>
@@ -414,7 +414,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.858883216167294E-09</v>
+        <v>0.0002195405251500087</v>
       </c>
       <c r="D2">
         <v>0.5847165279804634</v>
@@ -431,7 +431,7 @@
         <v>2.950586604829724E-10</v>
       </c>
       <c r="C3">
-        <v>0.0005025079404054473</v>
+        <v>0.01062411525673284</v>
       </c>
       <c r="D3">
         <v>0.5098564920815787</v>
@@ -448,7 +448,7 @@
         <v>4.605951621712099E-12</v>
       </c>
       <c r="C4">
-        <v>9.977804045657202E-05</v>
+        <v>0.009608716352691784</v>
       </c>
       <c r="D4">
         <v>0.4166937525759319</v>
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>4.627657735623706E-18</v>
+        <v>2.138791829054013E-07</v>
       </c>
       <c r="D5">
         <v>0.02303590698439988</v>
@@ -492,7 +492,7 @@
         <v>2011</v>
       </c>
       <c r="C1" s="1">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1">
         <v>2050</v>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.858883216167419E-09</v>
+        <v>0.0002195405251500235</v>
       </c>
       <c r="D2">
         <v>0.5847165279805026</v>
@@ -526,7 +526,7 @@
         <v>2.950586604829925E-10</v>
       </c>
       <c r="C3">
-        <v>0.0005025079404054812</v>
+        <v>0.01062411525673355</v>
       </c>
       <c r="D3">
         <v>0.5098564920816129</v>
@@ -543,7 +543,7 @@
         <v>4.60595162171241E-12</v>
       </c>
       <c r="C4">
-        <v>9.977804045657878E-05</v>
+        <v>0.009608716352692431</v>
       </c>
       <c r="D4">
         <v>0.41669375257596</v>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>4.627657735624077E-18</v>
+        <v>2.138791829054185E-07</v>
       </c>
       <c r="D5">
         <v>0.02303590698440173</v>
@@ -587,7 +587,7 @@
         <v>2011</v>
       </c>
       <c r="C1" s="1">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1">
         <v>2050</v>
@@ -604,7 +604,7 @@
         <v>9.901304551534366E-06</v>
       </c>
       <c r="C2">
-        <v>0.00045640749013724</v>
+        <v>0.007632681444695514</v>
       </c>
       <c r="D2">
         <v>1.101536214206334</v>
@@ -621,7 +621,7 @@
         <v>6.732543290709098E-05</v>
       </c>
       <c r="C3">
-        <v>0.02590083445439494</v>
+        <v>0.027535891297259</v>
       </c>
       <c r="D3">
         <v>0.782221375863945</v>
@@ -638,7 +638,7 @@
         <v>0.0001996663673797828</v>
       </c>
       <c r="C4">
-        <v>0.005661780233626572</v>
+        <v>0.007370778697872926</v>
       </c>
       <c r="D4">
         <v>0.6638415831600458</v>
@@ -655,7 +655,7 @@
         <v>6.272452008894037E-05</v>
       </c>
       <c r="C5">
-        <v>0.004141435196115032</v>
+        <v>0.016160587324431</v>
       </c>
       <c r="D5">
         <v>0.9533905590096068</v>
@@ -682,7 +682,7 @@
         <v>2011</v>
       </c>
       <c r="C1" s="1">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1">
         <v>2050</v>
@@ -699,7 +699,7 @@
         <v>8.265846938516411E-05</v>
       </c>
       <c r="C2">
-        <v>0.002352433236158991</v>
+        <v>0.005750015024097243</v>
       </c>
       <c r="D2">
         <v>1.548797540195856</v>
@@ -716,7 +716,7 @@
         <v>8.821213221951678E-05</v>
       </c>
       <c r="C3">
-        <v>0.04775458214733947</v>
+        <v>0.01921210602835477</v>
       </c>
       <c r="D3">
         <v>0.8156762103353417</v>
@@ -733,7 +733,7 @@
         <v>0.0005652393175857316</v>
       </c>
       <c r="C4">
-        <v>0.01052097936530436</v>
+        <v>0.0053924808017845</v>
       </c>
       <c r="D4">
         <v>0.8428959977190468</v>
@@ -750,7 +750,7 @@
         <v>0.0003035133465763992</v>
       </c>
       <c r="C5">
-        <v>0.01218230503195887</v>
+        <v>0.006847896595910315</v>
       </c>
       <c r="D5">
         <v>1.443724683792224</v>

</xml_diff>